<commit_message>
Added params_test.csv and functions_test.r
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -52,13 +52,13 @@
     <t xml:space="preserve">27.02.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">13.03.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.03.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.03.2020</t>
+    <t xml:space="preserve">07.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.03.2020</t>
   </si>
 </sst>
 </file>
@@ -158,10 +158,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
@@ -225,10 +225,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -242,7 +242,7 @@
         <v>0.01</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.05</v>
@@ -271,7 +271,7 @@
         <v>0.01</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1E-005</v>
+        <v>0.15</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0.05</v>

</xml_diff>

<commit_message>
pic defined on admission day
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -52,13 +52,13 @@
     <t xml:space="preserve">27.02.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">07.03.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.03.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.03.2020</t>
+    <t xml:space="preserve">13.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.03.2020</t>
   </si>
 </sst>
 </file>
@@ -158,10 +158,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
@@ -210,7 +210,7 @@
         <v>1.25</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.2</v>
@@ -225,10 +225,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,10 +239,10 @@
         <v>1.25</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.05</v>
@@ -254,10 +254,10 @@
         <v>12</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,11 +268,11 @@
         <v>1.12</v>
       </c>
       <c r="C4" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="D4" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0.15</v>
-      </c>
       <c r="E4" s="0" t="n">
         <v>0.05</v>
       </c>
@@ -283,10 +283,10 @@
         <v>12</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,7 +297,7 @@
         <v>1.12</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.05</v>
@@ -312,10 +312,10 @@
         <v>12</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pic at ICU entry + import individual data
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -64,16 +64,13 @@
     <t xml:space="preserve">Situation extraordinaire selon conseil fédéral</t>
   </si>
   <si>
-    <t xml:space="preserve">17.03.2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">21.03.2020</t>
   </si>
   <si>
     <t xml:space="preserve">28.03.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Début de l’effet du confinement (lam 1.15 → 1)</t>
+    <t xml:space="preserve">Début de l’effet du confinement (lam 1.12 → 1)</t>
   </si>
   <si>
     <t xml:space="preserve">05.04.2020</t>
@@ -191,13 +188,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
@@ -253,7 +250,7 @@
         <v>0.05</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0.1</v>
@@ -279,13 +276,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1.15</v>
+        <v>1.12</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.05</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0.1</v>
@@ -311,22 +308,22 @@
         <v>14</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1.15</v>
+        <v>1.12</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.05</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>12</v>
@@ -340,13 +337,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1.15</v>
+        <v>1.1</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0.05</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0.1</v>
@@ -362,20 +359,23 @@
       </c>
       <c r="I5" s="0" t="n">
         <v>50</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1.12</v>
+        <v>1.09</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0.05</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0.1</v>
@@ -391,9 +391,6 @@
       </c>
       <c r="I6" s="0" t="n">
         <v>50</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,7 +398,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1.1</v>
+        <v>1.08</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0.05</v>
@@ -430,7 +427,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1.08</v>
+        <v>1.05</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0.05</v>
@@ -459,7 +456,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1.05</v>
+        <v>1.02</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0.05</v>
@@ -488,7 +485,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0.05</v>
@@ -517,7 +514,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0.05</v>
@@ -540,37 +537,8 @@
       <c r="I11" s="0" t="n">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="J11" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
import.covid can load data.xlsx or individual patient data
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -191,10 +191,10 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>

</xml_diff>

<commit_message>
Add fit.nb function + update params.xlsx
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -191,10 +191,10 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
@@ -247,7 +247,7 @@
         <v>1.2</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.2</v>
@@ -259,13 +259,13 @@
         <v>2</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>11</v>
@@ -279,7 +279,7 @@
         <v>1.12</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.2</v>
@@ -291,13 +291,13 @@
         <v>2</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>13</v>
@@ -311,7 +311,7 @@
         <v>1.12</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.2</v>
@@ -323,13 +323,13 @@
         <v>2</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +340,7 @@
         <v>1.1</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.2</v>
@@ -352,13 +352,13 @@
         <v>2</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>16</v>
@@ -372,7 +372,7 @@
         <v>1.09</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0.2</v>
@@ -384,13 +384,13 @@
         <v>2</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,7 +401,7 @@
         <v>1.08</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0.2</v>
@@ -413,13 +413,13 @@
         <v>2</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,7 +430,7 @@
         <v>1.05</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0.2</v>
@@ -442,13 +442,13 @@
         <v>2</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +459,7 @@
         <v>1.02</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.2</v>
@@ -471,13 +471,13 @@
         <v>2</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +488,7 @@
         <v>1.01</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0.2</v>
@@ -500,13 +500,13 @@
         <v>2</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +517,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0.2</v>
@@ -529,13 +529,13 @@
         <v>2</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
New version with icp + adp
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -31,10 +31,16 @@
     <t xml:space="preserve">vlam</t>
   </si>
   <si>
-    <t xml:space="preserve">mpic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vpic</t>
+    <t xml:space="preserve">micp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vicp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">madp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vadp</t>
   </si>
   <si>
     <t xml:space="preserve">mlag</t>
@@ -188,23 +194,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="39.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,10 +244,16 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1.2</v>
@@ -256,24 +268,30 @@
         <v>0.1</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>154</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1.12</v>
@@ -288,24 +306,30 @@
         <v>0.1</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>154</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1.12</v>
@@ -320,21 +344,27 @@
         <v>0.1</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K4" s="0" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1.1</v>
@@ -349,24 +379,30 @@
         <v>0.1</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>154</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1.09</v>
@@ -381,21 +417,27 @@
         <v>0.1</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1.08</v>
@@ -410,21 +452,27 @@
         <v>0.1</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K7" s="0" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1.05</v>
@@ -439,21 +487,27 @@
         <v>0.1</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K8" s="0" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1.02</v>
@@ -468,21 +522,27 @@
         <v>0.1</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K9" s="0" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1.01</v>
@@ -497,21 +557,27 @@
         <v>0.1</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K10" s="0" t="n">
         <v>154</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -526,19 +592,25 @@
         <v>0.1</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>154</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>154</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename lam->egp and reformat date axis in plot.covid
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">mlam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vlam</t>
+    <t xml:space="preserve">megp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegp</t>
   </si>
   <si>
     <t xml:space="preserve">micp</t>
@@ -197,10 +197,10 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>

</xml_diff>

<commit_message>
Added predictions for nb of deaths
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -76,7 +76,7 @@
     <t xml:space="preserve">28.03.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Début de l’effet du confinement (lam 1.12 → 1)</t>
+    <t xml:space="preserve">Début de l’effet du confinement (egp 1.12 → 1)</t>
   </si>
   <si>
     <t xml:space="preserve">05.04.2020</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">15.05.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Fin supposée de l’épidémie (lam=1)</t>
+    <t xml:space="preserve">Fin supposée de l’épidémie (egp=1)</t>
   </si>
 </sst>
 </file>
@@ -197,10 +197,10 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.01"/>
@@ -332,7 +332,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1.12</v>
+        <v>1.05</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.08</v>
@@ -367,7 +367,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1.1</v>
+        <v>1.03</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0.08</v>
@@ -405,7 +405,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1.09</v>
+        <v>1.03</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0.08</v>
@@ -440,7 +440,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1.08</v>
+        <v>1.02</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0.08</v>
@@ -475,7 +475,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1.05</v>
+        <v>1.02</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0.08</v>
@@ -510,7 +510,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0.08</v>
@@ -545,7 +545,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1.01</v>
+        <v>1.005</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0.08</v>

</xml_diff>

<commit_message>
Mortality models adjusted for ic, age and sex
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="age_distrib" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="sex_distrib" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -119,17 +121,40 @@
   </si>
   <si>
     <t xml:space="preserve">Fin supposée de l’épidémie (megp=1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31-45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46-60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76-90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91-105</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -150,6 +175,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,13 +226,53 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -222,58 +294,54 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.28125" defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="5.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="5.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="39.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="3" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="70.65"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="s">
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -281,22 +349,22 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>1.2</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="C2" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -319,22 +387,22 @@
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>1.2</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="C3" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -353,26 +421,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="2" t="n">
         <v>1.12</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="n">
+      <c r="C4" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="0" t="n">
@@ -391,26 +459,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="2" t="n">
         <v>1.05</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="C5" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="0" t="n">
@@ -426,26 +494,26 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>1.03</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="0" t="n">
+      <c r="C6" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="0" t="n">
@@ -464,26 +532,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>1.03</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="C7" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="0" t="n">
@@ -499,26 +567,26 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="2" t="n">
         <v>1.02</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="0" t="n">
+      <c r="C8" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="0" t="n">
@@ -534,26 +602,26 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="2" t="n">
         <v>1.009</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="0" t="n">
+      <c r="C9" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="0" t="n">
@@ -569,26 +637,26 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="2" t="n">
         <v>1.01</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="0" t="n">
+      <c r="C10" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="0" t="n">
@@ -607,26 +675,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="2" t="n">
         <v>1.008</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="0" t="n">
+      <c r="C11" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="0" t="n">
@@ -642,26 +710,26 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="2" t="n">
         <v>1.012</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="0" t="n">
+      <c r="C12" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="0" t="n">
@@ -680,26 +748,26 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="2" t="n">
         <v>1.017</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="0" t="n">
+      <c r="C13" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="0" t="n">
@@ -718,26 +786,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="0" t="n">
+      <c r="B14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="0" t="n">
@@ -765,4 +833,171 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="7.65"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="D2" s="11" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E2" s="11" t="n">
+        <v>0.223</v>
+      </c>
+      <c r="F2" s="11" t="n">
+        <v>0.291</v>
+      </c>
+      <c r="G2" s="11" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="H2" s="11" t="n">
+        <v>0.062</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="7.65"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>0.458</v>
+      </c>
+      <c r="D2" s="11" t="n">
+        <v>0.478</v>
+      </c>
+      <c r="E2" s="11" t="n">
+        <v>0.349</v>
+      </c>
+      <c r="F2" s="11" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="G2" s="11" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="H2" s="11" t="n">
+        <v>0.514</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ICU restrictions on mortality
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -96,13 +96,13 @@
     <t xml:space="preserve">13.04.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">21.04.2020</t>
+    <t xml:space="preserve">23.04.2020</t>
   </si>
   <si>
     <t xml:space="preserve">Relâchement de pâques</t>
   </si>
   <si>
-    <t xml:space="preserve">24.04.2020</t>
+    <t xml:space="preserve">26.04.2020</t>
   </si>
   <si>
     <t xml:space="preserve">04.05.2020</t>
@@ -123,25 +123,13 @@
     <t xml:space="preserve">Fin supposée de l’épidémie (megp=1)</t>
   </si>
   <si>
-    <t xml:space="preserve">0-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31-45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46-60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61-75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76-90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91-105</t>
+    <t xml:space="preserve">0-64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65-74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75-104</t>
   </si>
 </sst>
 </file>
@@ -226,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -259,16 +247,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -294,13 +274,13 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="7.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="3" width="7.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="7.65"/>
@@ -356,7 +336,7 @@
         <v>0.08</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>0.1</v>
@@ -394,7 +374,7 @@
         <v>0.08</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>0.1</v>
@@ -432,7 +412,7 @@
         <v>0.08</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0.1</v>
@@ -470,7 +450,7 @@
         <v>0.08</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0.1</v>
@@ -505,7 +485,7 @@
         <v>0.08</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>0.1</v>
@@ -543,7 +523,7 @@
         <v>0.08</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>0.1</v>
@@ -578,7 +558,7 @@
         <v>0.08</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>0.1</v>
@@ -613,7 +593,7 @@
         <v>0.08</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>0.1</v>
@@ -642,13 +622,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>1.01</v>
+        <v>1.005</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0.08</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>0.1</v>
@@ -680,13 +660,13 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>1.008</v>
+        <v>1.005</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>0.08</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>0.1</v>
@@ -715,13 +695,13 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>1.012</v>
+        <v>1.006</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0.08</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>0.1</v>
@@ -753,13 +733,13 @@
         <v>29</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1.017</v>
+        <v>1.008</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>0.08</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>0.1</v>
@@ -797,7 +777,7 @@
         <v>0.08</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="E14" s="3" t="n">
         <v>0.1</v>
@@ -842,41 +822,34 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
@@ -886,30 +859,21 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="11" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="C2" s="11" t="n">
-        <v>0.021</v>
-      </c>
-      <c r="D2" s="11" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="E2" s="11" t="n">
-        <v>0.223</v>
-      </c>
-      <c r="F2" s="11" t="n">
-        <v>0.291</v>
-      </c>
-      <c r="G2" s="11" t="n">
-        <v>0.338</v>
-      </c>
-      <c r="H2" s="11" t="n">
-        <v>0.062</v>
-      </c>
+      <c r="B2" s="9" t="n">
+        <v>0.371</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -927,69 +891,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="7.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="7.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="11" t="n">
-        <v>0.458</v>
-      </c>
-      <c r="D2" s="11" t="n">
-        <v>0.478</v>
-      </c>
-      <c r="E2" s="11" t="n">
-        <v>0.349</v>
-      </c>
-      <c r="F2" s="11" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="G2" s="11" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="H2" s="11" t="n">
-        <v>0.514</v>
-      </c>
+      <c r="B2" s="9" t="n">
+        <v>0.368</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>0.372</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>0.469</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Updated survival models and new age categories
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -72,19 +72,28 @@
     <t xml:space="preserve">Début épidémie dans le canton de VD</t>
   </si>
   <si>
+    <t xml:space="preserve">28.02.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interdiction rassemblements &gt; 1000 personnes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interdiction rassemblements &gt; 100 personnes, fermeture écoles, contrôles aux frontières</t>
+  </si>
+  <si>
     <t xml:space="preserve">16.03.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Situation extraordinaire selon conseil fédéral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.03.2020</t>
+    <t xml:space="preserve">Situation extraordinaire : fermeture des commerces non essentiels, fermeture partielle des frontières</t>
   </si>
   <si>
     <t xml:space="preserve">28.03.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">Début de l’effet du confinement (megp 1.12 → 1)</t>
+    <t xml:space="preserve">Début de l’effet du confinement (megp → 1)</t>
   </si>
   <si>
     <t xml:space="preserve">05.04.2020</t>
@@ -93,43 +102,28 @@
     <t xml:space="preserve">10.04.2020</t>
   </si>
   <si>
-    <t xml:space="preserve">13.04.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.04.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relâchement de pâques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.04.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04.05.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relâchement des mesures (step 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.05.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relâchement des mesures (step 2 avec lag)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.09.2020</t>
+    <t xml:space="preserve">15.04.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.05.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.05.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.06.2020</t>
   </si>
   <si>
     <t xml:space="preserve">Fin supposée de l’épidémie (megp=1)</t>
   </si>
   <si>
-    <t xml:space="preserve">0-64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65-74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75-104</t>
+    <t xml:space="preserve">0-69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70-84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85-119</t>
   </si>
 </sst>
 </file>
@@ -272,19 +266,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="7.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="3" width="7.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="7.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="70.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="86.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,7 +327,7 @@
         <v>1.2</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>0.2</v>
@@ -371,7 +365,7 @@
         <v>1.2</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>0.2</v>
@@ -406,10 +400,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1.12</v>
+        <v>1.19</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0.2</v>
@@ -444,13 +438,13 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1.05</v>
+        <v>1.18</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0.1</v>
@@ -472,20 +466,23 @@
       </c>
       <c r="K5" s="0" t="n">
         <v>154</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>1.03</v>
+        <v>1.17</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>0.1</v>
@@ -509,18 +506,18 @@
         <v>154</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>0.18</v>
@@ -546,19 +543,22 @@
       <c r="K7" s="0" t="n">
         <v>154</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>0.1</v>
@@ -584,13 +584,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1.009</v>
+        <v>1.02</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>0.19</v>
@@ -619,16 +619,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>1.005</v>
+        <v>1.01</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>0.1</v>
@@ -650,20 +650,17 @@
       </c>
       <c r="K10" s="0" t="n">
         <v>154</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1.005</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>0.2</v>
@@ -692,13 +689,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>1.006</v>
+        <v>1.002</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>0.2</v>
@@ -723,9 +720,6 @@
       </c>
       <c r="K12" s="0" t="n">
         <v>154</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,10 +727,10 @@
         <v>29</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>1.008</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>0.2</v>
@@ -764,44 +758,6 @@
       </c>
       <c r="L13" s="0" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E14" s="3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F14" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>154</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -823,10 +779,10 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="7.65"/>
@@ -838,13 +794,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -863,13 +819,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="9" t="n">
-        <v>0.371</v>
+        <v>0.494</v>
       </c>
       <c r="C2" s="9" t="n">
-        <v>0.205</v>
+        <v>0.332</v>
       </c>
       <c r="D2" s="9" t="n">
-        <v>0.424</v>
+        <v>0.174</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -897,7 +853,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="7.65"/>
@@ -908,13 +864,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -925,13 +881,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="9" t="n">
-        <v>0.368</v>
+        <v>0.372</v>
       </c>
       <c r="C2" s="9" t="n">
-        <v>0.372</v>
+        <v>0.411</v>
       </c>
       <c r="D2" s="9" t="n">
-        <v>0.469</v>
+        <v>0.528</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>

</xml_diff>